<commit_message>
corrigi erro na tabela
</commit_message>
<xml_diff>
--- a/depressao.xlsx
+++ b/depressao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Graduação\2° Semestre\Ciência dos Dados\P2_CienciaDados_2019.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\DataSci\P2_CienciaDados_2019.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E77DC7-3A9E-421E-B2B0-3F3141D6799A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C761F4FC-A3E9-4CD4-BEF9-E8758FE9AD36}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6045,7 +6045,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6100,6 +6100,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -17847,8 +17850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A295" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E301" sqref="E301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20631,7 +20634,7 @@
         <v>888</v>
       </c>
       <c r="F111" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G111" t="s">
         <v>349</v>
@@ -25399,7 +25402,7 @@
       <c r="D301" s="18">
         <v>43718.982928240737</v>
       </c>
-      <c r="E301" s="8" t="s">
+      <c r="E301" s="19" t="s">
         <v>1851</v>
       </c>
       <c r="F301" s="13">

</xml_diff>